<commit_message>
Added fake challenge list to setup db script
</commit_message>
<xml_diff>
--- a/models/mock-data/MockChallengeList.xlsx
+++ b/models/mock-data/MockChallengeList.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -438,7 +438,7 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>